<commit_message>
Updated message sequence diagram. Added CONVEYOR_OCCUPIED and CONVEYOR_FREE to messages spreadsheet.
</commit_message>
<xml_diff>
--- a/docs/CAN Messages.xlsx
+++ b/docs/CAN Messages.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="51">
   <si>
     <t xml:space="preserve">Name</t>
   </si>
@@ -154,6 +154,18 @@
   </si>
   <si>
     <t xml:space="preserve">Sent when all components have indicated they are ready.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CONVEYOR_OCCUPIED</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sent when the conveyor is occupied</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CONVEYOR_FREE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sent when the conveyor is free.</t>
   </si>
   <si>
     <t xml:space="preserve">0x01</t>
@@ -278,15 +290,15 @@
   <dimension ref="A1:I25"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F16" activeCellId="0" sqref="F16"/>
+      <selection pane="topLeft" activeCell="F18" activeCellId="0" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="27.4030612244898"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.9591836734694"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="27.1326530612245"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.8265306122449"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -609,6 +621,46 @@
         <v>42</v>
       </c>
     </row>
+    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="B17" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="C17" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="D17" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="E17" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="F17" s="0" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="B18" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="C18" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="D18" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="E18" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="F18" s="0" t="s">
+        <v>46</v>
+      </c>
+    </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H21" s="0" t="s">
         <v>8</v>
@@ -616,7 +668,7 @@
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H22" s="0" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="I22" s="0" t="s">
         <v>12</v>
@@ -624,7 +676,7 @@
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H23" s="0" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="I23" s="0" t="s">
         <v>28</v>
@@ -632,7 +684,7 @@
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H24" s="0" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="I24" s="0" t="s">
         <v>25</v>
@@ -640,7 +692,7 @@
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H25" s="0" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="I25" s="0" t="s">
         <v>31</v>
@@ -670,7 +722,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -696,7 +748,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>